<commit_message>
Breitkopf all concertos changed to Orchestral
</commit_message>
<xml_diff>
--- a/Clear Music Time log 2021.xlsx
+++ b/Clear Music Time log 2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/keirenbrandt-sawdy/Documents/GitHub/Clearmusic-Publisher-Databases/Edited Files 28.07.21/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D588CCF8-3FD8-FA4B-918F-AC51ECAA0A1B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5551AD70-7283-964A-827C-C2EC266BC344}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4800" yWindow="500" windowWidth="28800" windowHeight="16500" xr2:uid="{546236D5-CC86-8E4E-BE32-7FD0F061102B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Date</t>
   </si>
@@ -40,6 +40,15 @@
   </si>
   <si>
     <t>Jo work</t>
+  </si>
+  <si>
+    <t>Amount paid by Clear Music</t>
+  </si>
+  <si>
+    <t>Hours Paid for</t>
+  </si>
+  <si>
+    <t>Hours left</t>
   </si>
 </sst>
 </file>
@@ -75,11 +84,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -395,15 +405,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F3BB817-8CDE-DD42-AEDD-F40082080526}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:D50"/>
+  <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="11" max="11" width="25.1640625" customWidth="1"/>
+    <col min="12" max="12" width="11.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -417,7 +431,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:12">
       <c r="A2" s="1">
         <v>44249</v>
       </c>
@@ -432,7 +446,7 @@
         <v>7.3611111111111072E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:12">
       <c r="A3" s="1">
         <v>44405</v>
       </c>
@@ -447,7 +461,7 @@
         <v>6.8749999999999978E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:12">
       <c r="A4" s="1">
         <v>44406</v>
       </c>
@@ -458,11 +472,11 @@
         <v>0.45555555555555555</v>
       </c>
       <c r="D4" s="2">
-        <f t="shared" ref="D4:D28" si="0">SUM(C4-B4)</f>
+        <f t="shared" ref="D4:D29" si="0">SUM(C4-B4)</f>
         <v>4.5138888888888895E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:12">
       <c r="A5" s="1">
         <v>44406</v>
       </c>
@@ -477,7 +491,7 @@
         <v>6.1111111111111172E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:12">
       <c r="A6" s="1">
         <v>44406</v>
       </c>
@@ -492,7 +506,7 @@
         <v>4.9999999999999933E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:12">
       <c r="A7" s="1">
         <v>44410</v>
       </c>
@@ -507,7 +521,7 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:12">
       <c r="A8" s="1">
         <v>44410</v>
       </c>
@@ -522,7 +536,7 @@
         <v>7.6388888888888618E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:12">
       <c r="A9" s="1">
         <v>44410</v>
       </c>
@@ -537,7 +551,7 @@
         <v>6.5277777777777768E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:12">
       <c r="A10" s="1">
         <v>44411</v>
       </c>
@@ -552,7 +566,7 @@
         <v>8.1944444444444431E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:12">
       <c r="A11" s="1">
         <v>44416</v>
       </c>
@@ -567,7 +581,7 @@
         <v>5.1388888888888873E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:12">
       <c r="A12" s="1">
         <v>44416</v>
       </c>
@@ -582,7 +596,7 @@
         <v>7.7777777777777724E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:12">
       <c r="A13" s="1">
         <v>44417</v>
       </c>
@@ -596,8 +610,14 @@
         <f t="shared" si="0"/>
         <v>4.1666666666666685E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="K13" t="s">
+        <v>5</v>
+      </c>
+      <c r="L13">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14" s="1">
         <v>44417</v>
       </c>
@@ -611,8 +631,15 @@
         <f t="shared" si="0"/>
         <v>1.8750000000000044E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="K14" t="s">
+        <v>6</v>
+      </c>
+      <c r="L14">
+        <f>L13/50</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15" s="1">
         <v>44418</v>
       </c>
@@ -626,8 +653,15 @@
         <f t="shared" si="0"/>
         <v>8.8194444444444409E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="K15" t="s">
+        <v>7</v>
+      </c>
+      <c r="L15" s="4">
+        <f>L14-36.5</f>
+        <v>23.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16" s="1">
         <v>44559</v>
       </c>
@@ -823,10 +857,19 @@
       </c>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="1"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
+      <c r="A29" s="1">
+        <v>44627</v>
+      </c>
+      <c r="B29" s="2">
+        <v>0.27291666666666664</v>
+      </c>
+      <c r="C29" s="2">
+        <v>0.27291666666666664</v>
+      </c>
+      <c r="D29" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="1"/>

</xml_diff>

<commit_message>
before editing the concerto instrumentation
</commit_message>
<xml_diff>
--- a/Clear Music Time log 2021.xlsx
+++ b/Clear Music Time log 2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/keirenbrandt-sawdy/Documents/GitHub/Clearmusic-Publisher-Databases/Edited Files 28.07.21/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3CC337F-4ADE-6F4F-B55E-CB49D1EDA9F0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{374517AA-17DD-D341-A2DA-E31F4819B44B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16500" xr2:uid="{546236D5-CC86-8E4E-BE32-7FD0F061102B}"/>
   </bookViews>
@@ -407,8 +407,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -891,11 +891,11 @@
         <v>0.375</v>
       </c>
       <c r="C31" s="2">
-        <v>0.375</v>
+        <v>0.5180555555555556</v>
       </c>
       <c r="D31" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.1430555555555556</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -962,7 +962,7 @@
       <c r="C42" s="2"/>
       <c r="D42" s="3">
         <f>SUM(D2:D41)</f>
-        <v>1.789583333333334</v>
+        <v>1.9326388888888895</v>
       </c>
     </row>
     <row r="43" spans="1:4">

</xml_diff>